<commit_message>
full c code for motor drivers to work with pwm
</commit_message>
<xml_diff>
--- a/Documents/SteperMotorCalcs.xlsx
+++ b/Documents/SteperMotorCalcs.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Macintosh HDD/Users/Jess/HDD Docs/ece492/capstoneMovingTarget/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF560BC9-1FA1-E14C-A7F9-308CECD88AF8}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{6F38EB86-6A73-004D-9B5F-9D34CFA99202}"/>
   </bookViews>
@@ -544,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87B386E3-4E58-7548-A126-95BB09C02335}">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -570,7 +571,7 @@
         <v>0.02</v>
       </c>
       <c r="F1" s="6">
-        <v>0.01</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="H1" s="6">
         <v>5.0000000000000001E-3</v>
@@ -731,7 +732,7 @@
       </c>
       <c r="F10" s="3">
         <f>F9*F1*1000</f>
-        <v>54.050000000000004</v>
+        <v>43.24</v>
       </c>
       <c r="G10" t="s">
         <v>4</v>
@@ -764,7 +765,7 @@
       </c>
       <c r="F11" s="1">
         <f>2*PI()*F1</f>
-        <v>6.2831853071795868E-2</v>
+        <v>5.0265482457436693E-2</v>
       </c>
       <c r="G11" t="s">
         <v>8</v>
@@ -797,7 +798,7 @@
       </c>
       <c r="F12" s="1">
         <f>F5/F11</f>
-        <v>3.9788735772973833</v>
+        <v>4.9735919716217287</v>
       </c>
       <c r="G12" t="s">
         <v>12</v>
@@ -830,7 +831,7 @@
       </c>
       <c r="F13">
         <f t="shared" ref="F13" si="0">F7*F12</f>
-        <v>1591.5494309189532</v>
+        <v>1989.4367886486914</v>
       </c>
       <c r="G13" t="s">
         <v>23</v>
@@ -859,7 +860,7 @@
       </c>
       <c r="F14">
         <f>F12/F6</f>
-        <v>6.1213439650728976</v>
+        <v>7.6516799563411206</v>
       </c>
       <c r="G14" t="s">
         <v>15</v>
@@ -892,7 +893,7 @@
       </c>
       <c r="F15">
         <f>F13/F6</f>
-        <v>2448.5375860291588</v>
+        <v>3060.671982536448</v>
       </c>
       <c r="G15" t="s">
         <v>18</v>
@@ -927,7 +928,7 @@
         <v>0.02</v>
       </c>
       <c r="F18" s="6">
-        <v>0.01</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="H18" s="6">
         <v>5.0000000000000001E-3</v>
@@ -1088,7 +1089,7 @@
       </c>
       <c r="F27" s="3">
         <f>F26*F18*1000</f>
-        <v>75.67</v>
+        <v>60.536000000000001</v>
       </c>
       <c r="G27" t="s">
         <v>4</v>
@@ -1121,7 +1122,7 @@
       </c>
       <c r="F28" s="1">
         <f>2*PI()*F18</f>
-        <v>6.2831853071795868E-2</v>
+        <v>5.0265482457436693E-2</v>
       </c>
       <c r="G28" t="s">
         <v>8</v>
@@ -1154,7 +1155,7 @@
       </c>
       <c r="F29" s="1">
         <f>F22/F28</f>
-        <v>3.9788735772973833</v>
+        <v>4.9735919716217287</v>
       </c>
       <c r="G29" t="s">
         <v>12</v>
@@ -1187,7 +1188,7 @@
       </c>
       <c r="F30">
         <f t="shared" ref="F30" si="1">F24*F29</f>
-        <v>1591.5494309189532</v>
+        <v>1989.4367886486914</v>
       </c>
       <c r="G30" t="s">
         <v>23</v>
@@ -1216,7 +1217,7 @@
       </c>
       <c r="F31">
         <f>F29/F23</f>
-        <v>6.1213439650728976</v>
+        <v>7.6516799563411206</v>
       </c>
       <c r="G31" t="s">
         <v>15</v>
@@ -1249,7 +1250,7 @@
       </c>
       <c r="F32">
         <f>F30/F23</f>
-        <v>2448.5375860291588</v>
+        <v>3060.671982536448</v>
       </c>
       <c r="G32" t="s">
         <v>18</v>
@@ -1284,7 +1285,7 @@
         <v>0.02</v>
       </c>
       <c r="F35" s="6">
-        <v>0.01</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="H35" s="6">
         <v>5.0000000000000001E-3</v>
@@ -1445,7 +1446,7 @@
       </c>
       <c r="F44" s="3">
         <f>F43*F35*1000</f>
-        <v>97.29000000000002</v>
+        <v>77.832000000000008</v>
       </c>
       <c r="G44" t="s">
         <v>4</v>
@@ -1478,7 +1479,7 @@
       </c>
       <c r="F45" s="1">
         <f>2*PI()*F35</f>
-        <v>6.2831853071795868E-2</v>
+        <v>5.0265482457436693E-2</v>
       </c>
       <c r="G45" t="s">
         <v>8</v>
@@ -1511,7 +1512,7 @@
       </c>
       <c r="F46" s="1">
         <f>F39/F45</f>
-        <v>3.9788735772973833</v>
+        <v>4.9735919716217287</v>
       </c>
       <c r="G46" t="s">
         <v>12</v>
@@ -1544,7 +1545,7 @@
       </c>
       <c r="F47">
         <f t="shared" ref="F47" si="2">F41*F46</f>
-        <v>1591.5494309189532</v>
+        <v>1989.4367886486914</v>
       </c>
       <c r="G47" t="s">
         <v>23</v>
@@ -1573,7 +1574,7 @@
       </c>
       <c r="F48">
         <f>F46/F40</f>
-        <v>6.1213439650728976</v>
+        <v>7.6516799563411206</v>
       </c>
       <c r="G48" t="s">
         <v>15</v>
@@ -1606,7 +1607,7 @@
       </c>
       <c r="F49">
         <f>F47/F40</f>
-        <v>2448.5375860291588</v>
+        <v>3060.671982536448</v>
       </c>
       <c r="G49" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
cleaning up PWM code for progress report
</commit_message>
<xml_diff>
--- a/Documents/SteperMotorCalcs.xlsx
+++ b/Documents/SteperMotorCalcs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Macintosh HDD/Users/Jess/HDD Docs/ece492/capstoneMovingTarget/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF560BC9-1FA1-E14C-A7F9-308CECD88AF8}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13DAE5E-4188-094B-8B41-C64E37C9BAFD}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{6F38EB86-6A73-004D-9B5F-9D34CFA99202}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{6F38EB86-6A73-004D-9B5F-9D34CFA99202}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="29">
   <si>
     <t>Radius (m)</t>
   </si>
@@ -107,6 +107,12 @@
   </si>
   <si>
     <t>associated torque is ~100mNm</t>
+  </si>
+  <si>
+    <t>2100 Pulses</t>
+  </si>
+  <si>
+    <t>4038 Pulses</t>
   </si>
 </sst>
 </file>
@@ -244,6 +250,1267 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Pulses Vs Time Graph (10%</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Ramp Up)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>3590 Pulses</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$C$3:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.5000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.19500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.32500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.45500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.58499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.65</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$D$3:$D$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3590</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3590</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3590</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3590</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3590</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3590</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3590</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3590</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3590</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FDB7-EB4C-AFBD-E0194CD4C694}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>2100 Pulses</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$C$3:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.5000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.19500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.32500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.45500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.58499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.65</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$E$3:$E$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FDB7-EB4C-AFBD-E0194CD4C694}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="625476111"/>
+        <c:axId val="705174447"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="625476111"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="705174447"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="705174447"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Pulses</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="625476111"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87043BB0-998B-0845-A2DF-01BC4F24794D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -545,7 +1812,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87B386E3-4E58-7548-A126-95BB09C02335}">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
@@ -1639,31 +2906,40 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{203AA49C-6852-6A45-8212-040E8B3250D1}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N34" sqref="N34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="15.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C1" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1">
+        <v>0.2</v>
+      </c>
+      <c r="I1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C2">
         <v>0.1</v>
       </c>
-      <c r="D2">
-        <v>0.2</v>
-      </c>
-      <c r="E2">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -1677,10 +2953,22 @@
         <v>0</v>
       </c>
       <c r="E3">
+        <v>2100</v>
+      </c>
+      <c r="F3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>2100</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>1</v>
       </c>
@@ -1689,15 +2977,27 @@
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="D4">
+        <v>3590</v>
+      </c>
+      <c r="E4">
+        <v>2100</v>
+      </c>
+      <c r="F4">
         <f>0.65*0.2*B4</f>
         <v>0.13</v>
       </c>
-      <c r="E4">
+      <c r="G4">
+        <v>4038</v>
+      </c>
+      <c r="H4">
+        <v>2100</v>
+      </c>
+      <c r="I4">
         <f>0.65*0.25*B4</f>
         <v>0.16250000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>2</v>
       </c>
@@ -1706,15 +3006,27 @@
         <v>0.13</v>
       </c>
       <c r="D5">
+        <v>3590</v>
+      </c>
+      <c r="E5">
+        <v>2100</v>
+      </c>
+      <c r="F5">
         <f>0.65*0.2*B5</f>
         <v>0.26</v>
       </c>
-      <c r="E5">
+      <c r="G5">
+        <v>4038</v>
+      </c>
+      <c r="H5">
+        <v>2100</v>
+      </c>
+      <c r="I5">
         <f>0.65*0.25*B5</f>
         <v>0.32500000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>3</v>
       </c>
@@ -1723,15 +3035,27 @@
         <v>0.19500000000000001</v>
       </c>
       <c r="D6">
+        <v>3590</v>
+      </c>
+      <c r="E6">
+        <v>2100</v>
+      </c>
+      <c r="F6">
         <f>0.65*0.2*B6</f>
         <v>0.39</v>
       </c>
-      <c r="E6">
+      <c r="G6">
+        <v>4038</v>
+      </c>
+      <c r="H6">
+        <v>2100</v>
+      </c>
+      <c r="I6">
         <f>0.65*0.25*B6</f>
         <v>0.48750000000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>4</v>
       </c>
@@ -1740,15 +3064,27 @@
         <v>0.26</v>
       </c>
       <c r="D7">
+        <v>3590</v>
+      </c>
+      <c r="E7">
+        <v>2100</v>
+      </c>
+      <c r="F7">
         <f>0.65*0.2*B7</f>
         <v>0.52</v>
       </c>
-      <c r="E7">
+      <c r="G7">
+        <v>4038</v>
+      </c>
+      <c r="H7">
+        <v>2100</v>
+      </c>
+      <c r="I7">
         <f>0.65*0.25*B7</f>
         <v>0.65</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>5</v>
       </c>
@@ -1757,11 +3093,23 @@
         <v>0.32500000000000001</v>
       </c>
       <c r="D8">
+        <v>3590</v>
+      </c>
+      <c r="E8">
+        <v>2100</v>
+      </c>
+      <c r="F8">
         <f>0.65*0.2*B8</f>
         <v>0.65</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>6</v>
       </c>
@@ -1769,8 +3117,14 @@
         <f t="shared" si="0"/>
         <v>0.39</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <v>3590</v>
+      </c>
+      <c r="E9">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>7</v>
       </c>
@@ -1778,8 +3132,14 @@
         <f t="shared" si="0"/>
         <v>0.45500000000000002</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <v>3590</v>
+      </c>
+      <c r="E10">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>8</v>
       </c>
@@ -1787,8 +3147,14 @@
         <f t="shared" si="0"/>
         <v>0.52</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <v>3590</v>
+      </c>
+      <c r="E11">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>9</v>
       </c>
@@ -1796,8 +3162,14 @@
         <f t="shared" si="0"/>
         <v>0.58499999999999996</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <v>3590</v>
+      </c>
+      <c r="E12">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B13">
         <v>10</v>
       </c>
@@ -1805,8 +3177,15 @@
         <f t="shared" si="0"/>
         <v>0.65</v>
       </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>2100</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>